<commit_message>
added Key Stages 1 - 4
</commit_message>
<xml_diff>
--- a/KS3/Year-7.xlsx
+++ b/KS3/Year-7.xlsx
@@ -199,13 +199,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> -I can describe what is meant by the term ‘fair use’
-- I can find copyright-free images
-- I can say why I should use copyright-free images  -I can add content to my own web page
-- I can evaluate what my web page looks like on different devices and suggest/make edits
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Learners should describe what is meant by term 'fair use'          Learners should find copyright-free images                             Learners should add content to their web page                                                         Learners should preview and evaluate their pages on different devices and make edits                                  </t>
   </si>
   <si>
@@ -400,6 +393,13 @@
   </si>
   <si>
     <t xml:space="preserve">Google Sites                                                                     Crystal Teachcomp </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -I can describe what is meant by the term ‘fair use’
+- I can find copyright-free images
+- I can say why I should use copyright-free images                                           -I can add content to my own web page
+- I can evaluate what my web page looks like on different devices and suggest/make edits
+</t>
   </si>
 </sst>
 </file>
@@ -937,9 +937,9 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="38.1" customHeight="1"/>
@@ -1020,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
@@ -1041,7 +1041,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>42</v>
@@ -1061,7 +1061,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>28</v>
@@ -1082,7 +1082,7 @@
         <v>39</v>
       </c>
       <c r="J4" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>43</v>
@@ -1102,7 +1102,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>28</v>
@@ -1123,7 +1123,7 @@
         <v>36</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>46</v>
@@ -1143,7 +1143,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>26</v>
@@ -1164,7 +1164,7 @@
         <v>35</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>48</v>
@@ -1184,7 +1184,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>26</v>
@@ -1205,13 +1205,13 @@
         <v>37</v>
       </c>
       <c r="J7" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="M7" s="10">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>26</v>
@@ -1246,13 +1246,13 @@
         <v>41</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="M8" s="10">
         <v>0</v>
@@ -1266,7 +1266,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>27</v>
@@ -1287,13 +1287,13 @@
         <v>38</v>
       </c>
       <c r="J9" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="M9" s="12">
         <v>1</v>
@@ -1307,7 +1307,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>27</v>
@@ -1328,10 +1328,10 @@
         <v>3</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>4</v>
@@ -1348,7 +1348,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>27</v>
@@ -1369,13 +1369,13 @@
         <v>5</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M11" s="3">
         <v>1</v>
@@ -1389,7 +1389,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>27</v>
@@ -1410,13 +1410,13 @@
         <v>6</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M12" s="3">
         <v>1</v>
@@ -1430,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>27</v>
@@ -1451,10 +1451,10 @@
         <v>7</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>8</v>
@@ -1471,7 +1471,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>27</v>
@@ -1489,16 +1489,16 @@
         <v>3</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="M14" s="6">
         <v>1</v>
@@ -1512,7 +1512,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>33</v>
@@ -1530,13 +1530,13 @@
         <v>1</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>9</v>
@@ -1553,7 +1553,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>33</v>
@@ -1571,13 +1571,13 @@
         <v>2</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>10</v>
@@ -1594,7 +1594,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>33</v>
@@ -1612,13 +1612,13 @@
         <v>3</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>11</v>
@@ -1635,7 +1635,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>33</v>
@@ -1653,16 +1653,16 @@
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="M18" s="3">
         <v>1</v>
@@ -1676,7 +1676,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>33</v>
@@ -1694,13 +1694,13 @@
         <v>2</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>12</v>
@@ -1717,7 +1717,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>33</v>
@@ -1735,16 +1735,16 @@
         <v>3</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K20" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="M20" s="6">
         <v>1</v>
@@ -1758,7 +1758,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>27</v>
@@ -1776,13 +1776,13 @@
         <v>1</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>13</v>
@@ -1799,7 +1799,7 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>27</v>
@@ -1817,16 +1817,16 @@
         <v>2</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M22" s="10">
         <v>0</v>
@@ -1840,7 +1840,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>27</v>
@@ -1858,16 +1858,16 @@
         <v>3</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M23" s="10">
         <v>0</v>
@@ -1881,7 +1881,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>27</v>
@@ -1899,13 +1899,13 @@
         <v>1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>14</v>
@@ -1922,7 +1922,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>27</v>
@@ -1940,16 +1940,16 @@
         <v>2</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M25" s="10">
         <v>0</v>
@@ -1963,7 +1963,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>27</v>
@@ -1981,13 +1981,13 @@
         <v>3</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>15</v>

</xml_diff>